<commit_message>
fixed my own bug <3
</commit_message>
<xml_diff>
--- a/Experiments/221227_Mdh/combined_sp_updated.xlsx
+++ b/Experiments/221227_Mdh/combined_sp_updated.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="97">
   <si>
     <t>PlateID</t>
   </si>
@@ -244,51 +244,51 @@
     <t>60</t>
   </si>
   <si>
-    <t>52.8,60.0,</t>
-  </si>
-  <si>
-    <t>54.0,60.0,</t>
+    <t>58.2,60.0,</t>
+  </si>
+  <si>
+    <t>58.5,60.0,</t>
+  </si>
+  <si>
+    <t>50.25,</t>
+  </si>
+  <si>
+    <t>52.5,60.0,60.0,60.0,60.0,60.0,</t>
+  </si>
+  <si>
+    <t>56.1,</t>
+  </si>
+  <si>
+    <t>44.4,60.0,</t>
+  </si>
+  <si>
+    <t>57.0,60.0,</t>
+  </si>
+  <si>
+    <t>60.0,60.0,60.0,</t>
+  </si>
+  <si>
+    <t>40.5,60.0,</t>
+  </si>
+  <si>
+    <t>60.0,52.0,53.0,</t>
+  </si>
+  <si>
+    <t>61.225,</t>
+  </si>
+  <si>
+    <t>35.25,</t>
+  </si>
+  <si>
+    <t>40.5,</t>
+  </si>
+  <si>
+    <t>60.0,60.0,</t>
   </si>
   <si>
     <t>48.0,</t>
   </si>
   <si>
-    <t>30.0,60.0,60.0,60.0,60.0,60.0,</t>
-  </si>
-  <si>
-    <t>55.199999999999996,</t>
-  </si>
-  <si>
-    <t>40.800000000000004,60.0,</t>
-  </si>
-  <si>
-    <t>48.0,60.0,</t>
-  </si>
-  <si>
-    <t>60.0,60.0,60.0,</t>
-  </si>
-  <si>
-    <t>36.0,60.0,</t>
-  </si>
-  <si>
-    <t>58.85,52.0,53.0,</t>
-  </si>
-  <si>
-    <t>60.075,</t>
-  </si>
-  <si>
-    <t>35.25,</t>
-  </si>
-  <si>
-    <t>36.0,</t>
-  </si>
-  <si>
-    <t>46.85,60.0,</t>
-  </si>
-  <si>
-    <t>60.0,60.0,</t>
-  </si>
-  <si>
     <t>57.0,</t>
   </si>
   <si>
@@ -301,13 +301,10 @@
     <t>60.0,</t>
   </si>
   <si>
-    <t>1763.65,2000.0,</t>
+    <t>1965.05,2000.0,</t>
   </si>
   <si>
     <t>52.5,</t>
-  </si>
-  <si>
-    <t>47.5,</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1059,7 @@
         <v>67</v>
       </c>
       <c r="H17" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1085,7 +1082,7 @@
         <v>73</v>
       </c>
       <c r="H18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1108,7 +1105,7 @@
         <v>48</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1266,7 +1263,7 @@
         <v>75</v>
       </c>
       <c r="H26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1312,7 +1309,7 @@
         <v>75</v>
       </c>
       <c r="H28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1335,7 +1332,7 @@
         <v>75</v>
       </c>
       <c r="H29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1358,7 +1355,7 @@
         <v>75</v>
       </c>
       <c r="H30" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>